<commit_message>
adding table for translation noise experiment
</commit_message>
<xml_diff>
--- a/results/NoiseTrans.xlsx
+++ b/results/NoiseTrans.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luke\Documents\GitHub\phdThesis\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="28620" windowHeight="12915" activeTab="3"/>
   </bookViews>
@@ -14,7 +19,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -636,6 +641,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -643,7 +651,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-AU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1228,11 +1236,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="113053056"/>
-        <c:axId val="113063424"/>
+        <c:axId val="188727768"/>
+        <c:axId val="188728552"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="113053056"/>
+        <c:axId val="188727768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1254,7 +1262,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1271,12 +1278,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113063424"/>
+        <c:crossAx val="188728552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="113063424"/>
+        <c:axId val="188728552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1299,7 +1306,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1316,14 +1322,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="113053056"/>
+        <c:crossAx val="188727768"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1346,7 +1351,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-AU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1931,11 +1936,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="139490432"/>
-        <c:axId val="139492352"/>
+        <c:axId val="190286032"/>
+        <c:axId val="190286424"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="139490432"/>
+        <c:axId val="190286032"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1957,7 +1962,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1974,12 +1978,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="139492352"/>
+        <c:crossAx val="190286424"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="139492352"/>
+        <c:axId val="190286424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2002,7 +2006,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2019,14 +2022,13 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="139490432"/>
+        <c:crossAx val="190286032"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -2049,7 +2051,7 @@
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-AU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2634,11 +2636,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="133875200"/>
-        <c:axId val="133877120"/>
+        <c:axId val="190286816"/>
+        <c:axId val="190287208"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="133875200"/>
+        <c:axId val="190286816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2660,19 +2662,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133877120"/>
+        <c:crossAx val="190287208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="133877120"/>
+        <c:axId val="190287208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2695,21 +2696,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133875200"/>
+        <c:crossAx val="190286816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -2742,7 +2741,7 @@
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-AU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -3327,11 +3326,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="38548224"/>
-        <c:axId val="38550528"/>
+        <c:axId val="190287600"/>
+        <c:axId val="190287992"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="38548224"/>
+        <c:axId val="190287600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3360,12 +3359,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38550528"/>
+        <c:crossAx val="190287992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="38550528"/>
+        <c:axId val="190287992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3395,7 +3394,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="38548224"/>
+        <c:crossAx val="190287600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3420,7 +3419,7 @@
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-AU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4005,11 +4004,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="41577088"/>
-        <c:axId val="41620992"/>
+        <c:axId val="190288776"/>
+        <c:axId val="190284464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="41577088"/>
+        <c:axId val="190288776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4038,12 +4037,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41620992"/>
+        <c:crossAx val="190284464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="41620992"/>
+        <c:axId val="190284464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4073,7 +4072,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41577088"/>
+        <c:crossAx val="190288776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4098,7 +4097,7 @@
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-AU"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -4683,11 +4682,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="94333184"/>
-        <c:axId val="41476096"/>
+        <c:axId val="190284856"/>
+        <c:axId val="190283288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="94333184"/>
+        <c:axId val="190284856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4716,12 +4715,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="41476096"/>
+        <c:crossAx val="190283288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="41476096"/>
+        <c:axId val="190283288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4751,7 +4750,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94333184"/>
+        <c:crossAx val="190284856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5032,7 +5031,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5067,7 +5066,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -5278,8 +5277,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L476"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="J46" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5572,7 +5571,28 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C16" s="24">
+        <f>AVERAGE(C3:C15)</f>
+        <v>100</v>
+      </c>
+      <c r="D16" s="24">
+        <f>AVERAGE(D3:D15)</f>
+        <v>100</v>
+      </c>
+      <c r="E16" s="24">
+        <f>AVERAGE(E3:E15)</f>
+        <v>23.829351992307693</v>
+      </c>
+      <c r="F16" s="24">
+        <f>AVERAGE(F3:F15)</f>
+        <v>100</v>
+      </c>
+      <c r="G16" s="24">
+        <f>AVERAGE(G3:G15)</f>
+        <v>100</v>
+      </c>
+    </row>
     <row r="17" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="24" t="s">
         <v>18</v>
@@ -5861,7 +5881,28 @@
         <v>100</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C32" s="24">
+        <f>AVERAGE(C19:C31)</f>
+        <v>100</v>
+      </c>
+      <c r="D32" s="24">
+        <f t="shared" ref="D32:G32" si="0">AVERAGE(D19:D31)</f>
+        <v>100</v>
+      </c>
+      <c r="E32" s="24">
+        <f t="shared" si="0"/>
+        <v>9.158654544615386</v>
+      </c>
+      <c r="F32" s="24">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="G32" s="24">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+    </row>
     <row r="33" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="34" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="35" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
@@ -6153,7 +6194,28 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="24">
+        <f>AVERAGE(C38:C50)</f>
+        <v>100</v>
+      </c>
+      <c r="D51" s="24">
+        <f>AVERAGE(D38:D50)</f>
+        <v>100</v>
+      </c>
+      <c r="E51" s="24">
+        <f>AVERAGE(E38:E50)</f>
+        <v>23.240760000000002</v>
+      </c>
+      <c r="F51" s="24">
+        <f>AVERAGE(F38:F50)</f>
+        <v>100</v>
+      </c>
+      <c r="G51" s="24">
+        <f>AVERAGE(G38:G50)</f>
+        <v>100</v>
+      </c>
+    </row>
     <row r="52" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="53" spans="1:12" s="24" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="55" spans="1:12" x14ac:dyDescent="0.25">

</xml_diff>